<commit_message>
ETL for target added, DLM updated
</commit_message>
<xml_diff>
--- a/02/DLM/DLM.xlsx
+++ b/02/DLM/DLM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\EDW\semestralWork\mi-edw-2020-chvostom\02\DLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B490DDD3-90C6-4864-9FE9-F5D2AABC277A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EE9548-7B4D-4C7D-A2B0-14AFF6774FF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{8B3B546D-74BE-4BB6-9CE3-13489F60C3E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="246">
   <si>
     <t>Entita</t>
   </si>
@@ -607,6 +607,162 @@
   </si>
   <si>
     <t>Typ SCD</t>
+  </si>
+  <si>
+    <t>t_account_LOAD</t>
+  </si>
+  <si>
+    <t>t_credit_card_LOAD</t>
+  </si>
+  <si>
+    <t>t_client_LOAD</t>
+  </si>
+  <si>
+    <t>t_disposition_LOAD</t>
+  </si>
+  <si>
+    <t>t_district_LOAD</t>
+  </si>
+  <si>
+    <t>t_loan_LOAD</t>
+  </si>
+  <si>
+    <t>t_permanent_order_LOAD</t>
+  </si>
+  <si>
+    <t>t_transaction_LOAD</t>
+  </si>
+  <si>
+    <t>ucet_id</t>
+  </si>
+  <si>
+    <t>okres_id</t>
+  </si>
+  <si>
+    <t>dispozice_id</t>
+  </si>
+  <si>
+    <t>klient_id</t>
+  </si>
+  <si>
+    <t>uctovaci_obdobi</t>
+  </si>
+  <si>
+    <t>datum_vytvoreni</t>
+  </si>
+  <si>
+    <t>karta_id</t>
+  </si>
+  <si>
+    <t>karta_typ</t>
+  </si>
+  <si>
+    <t>datum_vydani</t>
+  </si>
+  <si>
+    <t>rodne_cislo</t>
+  </si>
+  <si>
+    <t>klient_role</t>
+  </si>
+  <si>
+    <t>okres_nazev</t>
+  </si>
+  <si>
+    <t>region_nazev</t>
+  </si>
+  <si>
+    <t>pocet_obyvatel</t>
+  </si>
+  <si>
+    <t>obce_pod_500_obyvatel</t>
+  </si>
+  <si>
+    <t>obce_pod_2000_obyvatel</t>
+  </si>
+  <si>
+    <t>obce_pod_10000_obyvatel</t>
+  </si>
+  <si>
+    <t>obce_nad_10000_obyvatel</t>
+  </si>
+  <si>
+    <t>pocet_mest</t>
+  </si>
+  <si>
+    <t>prumerny_plat</t>
+  </si>
+  <si>
+    <t>nezamestnanost_1995</t>
+  </si>
+  <si>
+    <t>nezamestnanost_1996</t>
+  </si>
+  <si>
+    <t>pocet_podnikatelu</t>
+  </si>
+  <si>
+    <t>kriminalita_1995</t>
+  </si>
+  <si>
+    <t>kriminalita_1996</t>
+  </si>
+  <si>
+    <t>pujcka_id</t>
+  </si>
+  <si>
+    <t>datum_sjednani</t>
+  </si>
+  <si>
+    <t>castka</t>
+  </si>
+  <si>
+    <t>vyse_pujcky</t>
+  </si>
+  <si>
+    <t>doba_pujcky</t>
+  </si>
+  <si>
+    <t>vyse_splatky</t>
+  </si>
+  <si>
+    <t>stav_pujcky</t>
+  </si>
+  <si>
+    <t>platebni_prikaz_id</t>
+  </si>
+  <si>
+    <t>banka_prijemce</t>
+  </si>
+  <si>
+    <t>ucet_prijemce</t>
+  </si>
+  <si>
+    <t>platba_typ</t>
+  </si>
+  <si>
+    <t>transakce_id</t>
+  </si>
+  <si>
+    <t>datum_transakce</t>
+  </si>
+  <si>
+    <t>transakce_typ</t>
+  </si>
+  <si>
+    <t>transakce_operace</t>
+  </si>
+  <si>
+    <t>zustatek</t>
+  </si>
+  <si>
+    <t>transakce_info</t>
+  </si>
+  <si>
+    <t>banka_partnera</t>
+  </si>
+  <si>
+    <t>ucet_partnera</t>
   </si>
 </sst>
 </file>
@@ -967,6 +1123,15 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -988,12 +1153,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1009,13 +1168,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1341,7 +1497,7 @@
   <dimension ref="A1:LF1500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1358,9 +1514,9 @@
     <col min="10" max="10" width="20" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.88671875" style="1" customWidth="1"/>
     <col min="12" max="12" width="17.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="19.77734375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="41.44140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="65.109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="22.5546875" style="1" customWidth="1"/>
@@ -1388,35 +1544,35 @@
     </row>
     <row r="2" spans="1:318" s="12" customFormat="1" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="44" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="47"/>
       <c r="M2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42" t="s">
+      <c r="O2" s="42"/>
+      <c r="P2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="31" t="s">
+      <c r="Q2" s="44"/>
+      <c r="R2" s="34" t="s">
         <v>16</v>
       </c>
       <c r="S2" s="28"/>
@@ -1721,7 +1877,7 @@
       <c r="LF2" s="28"/>
     </row>
     <row r="3" spans="1:318" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +1923,7 @@
       <c r="Q3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="32"/>
+      <c r="R3" s="35"/>
     </row>
     <row r="4" spans="1:318" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -1803,11 +1959,15 @@
       <c r="L4" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="N4" s="16">
         <v>1</v>
       </c>
-      <c r="O4" s="18"/>
+      <c r="O4" s="18" t="s">
+        <v>194</v>
+      </c>
       <c r="P4" s="16" t="s">
         <v>70</v>
       </c>
@@ -1850,11 +2010,15 @@
       <c r="L5" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M5" s="14"/>
+      <c r="M5" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="N5" s="19">
         <v>1</v>
       </c>
-      <c r="O5" s="21"/>
+      <c r="O5" s="21" t="s">
+        <v>194</v>
+      </c>
       <c r="P5" s="19" t="s">
         <v>94</v>
       </c>
@@ -1897,11 +2061,15 @@
       <c r="L6" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="14" t="s">
+        <v>206</v>
+      </c>
       <c r="N6" s="19">
         <v>1</v>
       </c>
-      <c r="O6" s="21"/>
+      <c r="O6" s="21" t="s">
+        <v>194</v>
+      </c>
       <c r="P6" s="19" t="s">
         <v>71</v>
       </c>
@@ -1944,11 +2112,15 @@
       <c r="L7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="15"/>
+      <c r="M7" s="15" t="s">
+        <v>207</v>
+      </c>
       <c r="N7" s="22">
         <v>1</v>
       </c>
-      <c r="O7" s="23"/>
+      <c r="O7" s="23" t="s">
+        <v>194</v>
+      </c>
       <c r="P7" s="22" t="s">
         <v>72</v>
       </c>
@@ -1993,9 +2165,14 @@
       <c r="L8" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M8" s="24"/>
+      <c r="M8" s="24" t="s">
+        <v>208</v>
+      </c>
       <c r="N8" s="1">
         <v>1</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>75</v>
@@ -2025,7 +2202,7 @@
         <v>174</v>
       </c>
       <c r="H9" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>175</v>
@@ -2039,9 +2216,14 @@
       <c r="L9" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="14" t="s">
+        <v>204</v>
+      </c>
       <c r="N9" s="1">
         <v>1</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="P9" s="19" t="s">
         <v>76</v>
@@ -2071,7 +2253,7 @@
         <v>174</v>
       </c>
       <c r="H10" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>175</v>
@@ -2085,9 +2267,14 @@
       <c r="L10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="14" t="s">
+        <v>209</v>
+      </c>
       <c r="N10" s="1">
         <v>1</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="P10" s="19" t="s">
         <v>78</v>
@@ -2117,7 +2304,7 @@
         <v>174</v>
       </c>
       <c r="H11" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>175</v>
@@ -2131,11 +2318,15 @@
       <c r="L11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="15"/>
+      <c r="M11" s="15" t="s">
+        <v>210</v>
+      </c>
       <c r="N11" s="11">
         <v>1</v>
       </c>
-      <c r="O11" s="11"/>
+      <c r="O11" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="P11" s="22" t="s">
         <v>81</v>
       </c>
@@ -2180,9 +2371,14 @@
       <c r="L12" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="M12" s="14"/>
+      <c r="M12" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="N12" s="1">
         <v>1</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="P12" s="19" t="s">
         <v>84</v>
@@ -2212,7 +2408,7 @@
         <v>174</v>
       </c>
       <c r="H13" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>175</v>
@@ -2226,9 +2422,14 @@
       <c r="L13" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="M13" s="14"/>
+      <c r="M13" s="14" t="s">
+        <v>211</v>
+      </c>
       <c r="N13" s="1">
         <v>1</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="P13" s="19" t="s">
         <v>85</v>
@@ -2272,9 +2473,14 @@
       <c r="L14" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="M14" s="14"/>
+      <c r="M14" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="N14" s="1">
         <v>1</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="P14" s="22" t="s">
         <v>95</v>
@@ -2320,11 +2526,15 @@
       <c r="L15" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="24"/>
+      <c r="M15" s="24" t="s">
+        <v>204</v>
+      </c>
       <c r="N15" s="17">
         <v>1</v>
       </c>
-      <c r="O15" s="17"/>
+      <c r="O15" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="P15" s="19" t="s">
         <v>87</v>
       </c>
@@ -2367,11 +2577,15 @@
       <c r="L16" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M16" s="14"/>
+      <c r="M16" s="14" t="s">
+        <v>205</v>
+      </c>
       <c r="N16" s="20">
         <v>1</v>
       </c>
-      <c r="O16" s="20"/>
+      <c r="O16" s="20" t="s">
+        <v>197</v>
+      </c>
       <c r="P16" s="19" t="s">
         <v>88</v>
       </c>
@@ -2414,11 +2628,15 @@
       <c r="L17" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M17" s="14"/>
+      <c r="M17" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="N17" s="20">
         <v>1</v>
       </c>
-      <c r="O17" s="20"/>
+      <c r="O17" s="20" t="s">
+        <v>197</v>
+      </c>
       <c r="P17" s="19" t="s">
         <v>89</v>
       </c>
@@ -2461,11 +2679,15 @@
       <c r="L18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="15"/>
+      <c r="M18" s="15" t="s">
+        <v>212</v>
+      </c>
       <c r="N18" s="11">
         <v>1</v>
       </c>
-      <c r="O18" s="11"/>
+      <c r="O18" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="P18" s="22" t="s">
         <v>92</v>
       </c>
@@ -2510,9 +2732,14 @@
       <c r="L19" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="M19" s="14"/>
+      <c r="M19" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="N19" s="1">
         <v>1</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P19" s="19" t="s">
         <v>126</v>
@@ -2542,7 +2769,7 @@
         <v>174</v>
       </c>
       <c r="H20" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" s="19" t="s">
         <v>175</v>
@@ -2556,9 +2783,14 @@
       <c r="L20" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="14"/>
+      <c r="M20" s="14" t="s">
+        <v>213</v>
+      </c>
       <c r="N20" s="1">
         <v>1</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P20" s="19" t="s">
         <v>96</v>
@@ -2588,7 +2820,7 @@
         <v>174</v>
       </c>
       <c r="H21" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>175</v>
@@ -2602,9 +2834,14 @@
       <c r="L21" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="14"/>
+      <c r="M21" s="14" t="s">
+        <v>214</v>
+      </c>
       <c r="N21" s="1">
         <v>1</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P21" s="19" t="s">
         <v>97</v>
@@ -2634,7 +2871,7 @@
         <v>174</v>
       </c>
       <c r="H22" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>175</v>
@@ -2648,9 +2885,14 @@
       <c r="L22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M22" s="14"/>
+      <c r="M22" s="14" t="s">
+        <v>215</v>
+      </c>
       <c r="N22" s="1">
         <v>1</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P22" s="19" t="s">
         <v>105</v>
@@ -2680,7 +2922,7 @@
         <v>174</v>
       </c>
       <c r="H23" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>175</v>
@@ -2694,9 +2936,14 @@
       <c r="L23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="14"/>
+      <c r="M23" s="14" t="s">
+        <v>216</v>
+      </c>
       <c r="N23" s="1">
         <v>1</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P23" s="19" t="s">
         <v>107</v>
@@ -2726,7 +2973,7 @@
         <v>174</v>
       </c>
       <c r="H24" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>175</v>
@@ -2740,9 +2987,14 @@
       <c r="L24" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="14"/>
+      <c r="M24" s="14" t="s">
+        <v>217</v>
+      </c>
       <c r="N24" s="1">
         <v>1</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P24" s="19" t="s">
         <v>108</v>
@@ -2772,7 +3024,7 @@
         <v>174</v>
       </c>
       <c r="H25" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>175</v>
@@ -2786,9 +3038,14 @@
       <c r="L25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="14"/>
+      <c r="M25" s="14" t="s">
+        <v>218</v>
+      </c>
       <c r="N25" s="1">
         <v>1</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P25" s="19" t="s">
         <v>109</v>
@@ -2818,7 +3075,7 @@
         <v>174</v>
       </c>
       <c r="H26" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>175</v>
@@ -2832,9 +3089,14 @@
       <c r="L26" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="14"/>
+      <c r="M26" s="14" t="s">
+        <v>219</v>
+      </c>
       <c r="N26" s="1">
         <v>1</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P26" s="19" t="s">
         <v>110</v>
@@ -2864,7 +3126,7 @@
         <v>174</v>
       </c>
       <c r="H27" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>175</v>
@@ -2878,9 +3140,14 @@
       <c r="L27" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="14"/>
+      <c r="M27" s="14" t="s">
+        <v>220</v>
+      </c>
       <c r="N27" s="1">
         <v>1</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P27" s="19" t="s">
         <v>106</v>
@@ -2910,7 +3177,7 @@
         <v>174</v>
       </c>
       <c r="H28" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="19" t="s">
         <v>175</v>
@@ -2924,9 +3191,14 @@
       <c r="L28" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="M28" s="14"/>
+      <c r="M28" s="14" t="s">
+        <v>112</v>
+      </c>
       <c r="N28" s="1">
         <v>1</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P28" s="19" t="s">
         <v>112</v>
@@ -2956,7 +3228,7 @@
         <v>174</v>
       </c>
       <c r="H29" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>175</v>
@@ -2970,9 +3242,14 @@
       <c r="L29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="14"/>
+      <c r="M29" s="14" t="s">
+        <v>221</v>
+      </c>
       <c r="N29" s="1">
         <v>1</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P29" s="19" t="s">
         <v>114</v>
@@ -3016,9 +3293,14 @@
       <c r="L30" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="M30" s="14"/>
+      <c r="M30" s="14" t="s">
+        <v>222</v>
+      </c>
       <c r="N30" s="1">
         <v>1</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P30" s="19" t="s">
         <v>116</v>
@@ -3062,9 +3344,14 @@
       <c r="L31" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="M31" s="14"/>
+      <c r="M31" s="14" t="s">
+        <v>223</v>
+      </c>
       <c r="N31" s="1">
         <v>1</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P31" s="19" t="s">
         <v>117</v>
@@ -3094,7 +3381,7 @@
         <v>174</v>
       </c>
       <c r="H32" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>175</v>
@@ -3108,9 +3395,14 @@
       <c r="L32" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M32" s="14"/>
+      <c r="M32" s="14" t="s">
+        <v>224</v>
+      </c>
       <c r="N32" s="1">
         <v>1</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P32" s="19" t="s">
         <v>120</v>
@@ -3154,9 +3446,14 @@
       <c r="L33" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M33" s="14"/>
+      <c r="M33" s="14" t="s">
+        <v>225</v>
+      </c>
       <c r="N33" s="1">
         <v>1</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P33" s="19" t="s">
         <v>122</v>
@@ -3200,9 +3497,14 @@
       <c r="L34" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="M34" s="14"/>
+      <c r="M34" s="14" t="s">
+        <v>226</v>
+      </c>
       <c r="N34" s="1">
         <v>1</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="P34" s="19" t="s">
         <v>123</v>
@@ -3248,11 +3550,15 @@
       <c r="L35" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M35" s="24"/>
+      <c r="M35" s="24" t="s">
+        <v>227</v>
+      </c>
       <c r="N35" s="17">
         <v>1</v>
       </c>
-      <c r="O35" s="17"/>
+      <c r="O35" s="17" t="s">
+        <v>199</v>
+      </c>
       <c r="P35" s="16" t="s">
         <v>128</v>
       </c>
@@ -3281,7 +3587,7 @@
         <v>174</v>
       </c>
       <c r="H36" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>175</v>
@@ -3295,11 +3601,15 @@
       <c r="L36" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="M36" s="14"/>
+      <c r="M36" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="N36" s="20">
         <v>1</v>
       </c>
-      <c r="O36" s="20"/>
+      <c r="O36" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="P36" s="19" t="s">
         <v>129</v>
       </c>
@@ -3328,7 +3638,7 @@
         <v>174</v>
       </c>
       <c r="H37" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I37" s="19" t="s">
         <v>175</v>
@@ -3342,11 +3652,15 @@
       <c r="L37" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M37" s="14"/>
+      <c r="M37" s="14" t="s">
+        <v>228</v>
+      </c>
       <c r="N37" s="20">
         <v>1</v>
       </c>
-      <c r="O37" s="20"/>
+      <c r="O37" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="P37" s="19" t="s">
         <v>130</v>
       </c>
@@ -3375,7 +3689,7 @@
         <v>174</v>
       </c>
       <c r="H38" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I38" s="19" t="s">
         <v>175</v>
@@ -3389,11 +3703,15 @@
       <c r="L38" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M38" s="14"/>
+      <c r="M38" s="14" t="s">
+        <v>230</v>
+      </c>
       <c r="N38" s="20">
         <v>1</v>
       </c>
-      <c r="O38" s="20"/>
+      <c r="O38" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="P38" s="19" t="s">
         <v>132</v>
       </c>
@@ -3436,11 +3754,15 @@
       <c r="L39" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M39" s="14"/>
+      <c r="M39" s="14" t="s">
+        <v>231</v>
+      </c>
       <c r="N39" s="20">
         <v>1</v>
       </c>
-      <c r="O39" s="20"/>
+      <c r="O39" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="P39" s="19" t="s">
         <v>134</v>
       </c>
@@ -3483,11 +3805,15 @@
       <c r="L40" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="M40" s="14"/>
+      <c r="M40" s="14" t="s">
+        <v>232</v>
+      </c>
       <c r="N40" s="20">
         <v>1</v>
       </c>
-      <c r="O40" s="20"/>
+      <c r="O40" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="P40" s="19" t="s">
         <v>136</v>
       </c>
@@ -3530,11 +3856,15 @@
       <c r="L41" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="M41" s="15"/>
+      <c r="M41" s="15" t="s">
+        <v>233</v>
+      </c>
       <c r="N41" s="11">
         <v>1</v>
       </c>
-      <c r="O41" s="11"/>
+      <c r="O41" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="P41" s="22" t="s">
         <v>138</v>
       </c>
@@ -3579,9 +3909,14 @@
       <c r="L42" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="M42" s="14"/>
+      <c r="M42" s="14" t="s">
+        <v>234</v>
+      </c>
       <c r="N42" s="1">
         <v>1</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="P42" s="19" t="s">
         <v>140</v>
@@ -3625,9 +3960,14 @@
       <c r="L43" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M43" s="14"/>
+      <c r="M43" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="N43" s="1">
         <v>1</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="P43" s="19" t="s">
         <v>148</v>
@@ -3671,9 +4011,14 @@
       <c r="L44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M44" s="14"/>
+      <c r="M44" s="14" t="s">
+        <v>235</v>
+      </c>
       <c r="N44" s="1">
         <v>1</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="P44" s="19" t="s">
         <v>141</v>
@@ -3717,9 +4062,14 @@
       <c r="L45" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M45" s="14"/>
+      <c r="M45" s="14" t="s">
+        <v>236</v>
+      </c>
       <c r="N45" s="1">
         <v>1</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="P45" s="19" t="s">
         <v>142</v>
@@ -3763,9 +4113,14 @@
       <c r="L46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M46" s="14"/>
+      <c r="M46" s="14" t="s">
+        <v>229</v>
+      </c>
       <c r="N46" s="1">
         <v>1</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="P46" s="19" t="s">
         <v>156</v>
@@ -3809,9 +4164,14 @@
       <c r="L47" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="M47" s="14"/>
+      <c r="M47" s="14" t="s">
+        <v>237</v>
+      </c>
       <c r="N47" s="1">
         <v>1</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="P47" s="19" t="s">
         <v>144</v>
@@ -3857,11 +4217,15 @@
       <c r="L48" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M48" s="24"/>
+      <c r="M48" s="24" t="s">
+        <v>238</v>
+      </c>
       <c r="N48" s="17">
         <v>1</v>
       </c>
-      <c r="O48" s="17"/>
+      <c r="O48" s="17" t="s">
+        <v>201</v>
+      </c>
       <c r="P48" s="16" t="s">
         <v>146</v>
       </c>
@@ -3890,7 +4254,7 @@
         <v>174</v>
       </c>
       <c r="H49" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="20" t="s">
         <v>175</v>
@@ -3904,11 +4268,15 @@
       <c r="L49" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="M49" s="14"/>
+      <c r="M49" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="N49" s="20">
         <v>1</v>
       </c>
-      <c r="O49" s="20"/>
+      <c r="O49" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P49" s="19" t="s">
         <v>147</v>
       </c>
@@ -3937,7 +4305,7 @@
         <v>174</v>
       </c>
       <c r="H50" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="20" t="s">
         <v>175</v>
@@ -3951,11 +4319,15 @@
       <c r="L50" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M50" s="14"/>
+      <c r="M50" s="14" t="s">
+        <v>239</v>
+      </c>
       <c r="N50" s="20">
         <v>1</v>
       </c>
-      <c r="O50" s="20"/>
+      <c r="O50" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P50" s="19" t="s">
         <v>149</v>
       </c>
@@ -3984,7 +4356,7 @@
         <v>174</v>
       </c>
       <c r="H51" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="20" t="s">
         <v>175</v>
@@ -3998,11 +4370,15 @@
       <c r="L51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M51" s="14"/>
+      <c r="M51" s="14" t="s">
+        <v>240</v>
+      </c>
       <c r="N51" s="20">
         <v>1</v>
       </c>
-      <c r="O51" s="20"/>
+      <c r="O51" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P51" s="19" t="s">
         <v>151</v>
       </c>
@@ -4031,7 +4407,7 @@
         <v>174</v>
       </c>
       <c r="H52" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="20" t="s">
         <v>175</v>
@@ -4045,11 +4421,15 @@
       <c r="L52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M52" s="14"/>
+      <c r="M52" s="14" t="s">
+        <v>241</v>
+      </c>
       <c r="N52" s="20">
         <v>1</v>
       </c>
-      <c r="O52" s="20"/>
+      <c r="O52" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P52" s="19" t="s">
         <v>153</v>
       </c>
@@ -4078,7 +4458,7 @@
         <v>174</v>
       </c>
       <c r="H53" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="20" t="s">
         <v>175</v>
@@ -4092,11 +4472,15 @@
       <c r="L53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M53" s="14"/>
+      <c r="M53" s="14" t="s">
+        <v>229</v>
+      </c>
       <c r="N53" s="20">
         <v>1</v>
       </c>
-      <c r="O53" s="20"/>
+      <c r="O53" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P53" s="19" t="s">
         <v>155</v>
       </c>
@@ -4125,7 +4509,7 @@
         <v>174</v>
       </c>
       <c r="H54" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="20" t="s">
         <v>175</v>
@@ -4139,11 +4523,15 @@
       <c r="L54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M54" s="14"/>
+      <c r="M54" s="14" t="s">
+        <v>242</v>
+      </c>
       <c r="N54" s="20">
         <v>1</v>
       </c>
-      <c r="O54" s="20"/>
+      <c r="O54" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P54" s="19" t="s">
         <v>158</v>
       </c>
@@ -4172,7 +4560,7 @@
         <v>174</v>
       </c>
       <c r="H55" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="20" t="s">
         <v>175</v>
@@ -4186,11 +4574,15 @@
       <c r="L55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M55" s="14"/>
+      <c r="M55" s="14" t="s">
+        <v>243</v>
+      </c>
       <c r="N55" s="20">
         <v>1</v>
       </c>
-      <c r="O55" s="20"/>
+      <c r="O55" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P55" s="19" t="s">
         <v>160</v>
       </c>
@@ -4219,7 +4611,7 @@
         <v>174</v>
       </c>
       <c r="H56" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="20" t="s">
         <v>175</v>
@@ -4233,11 +4625,15 @@
       <c r="L56" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M56" s="14"/>
+      <c r="M56" s="14" t="s">
+        <v>244</v>
+      </c>
       <c r="N56" s="20">
         <v>1</v>
       </c>
-      <c r="O56" s="20"/>
+      <c r="O56" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P56" s="19" t="s">
         <v>162</v>
       </c>
@@ -4266,7 +4662,7 @@
         <v>174</v>
       </c>
       <c r="H57" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>175</v>
@@ -4280,11 +4676,15 @@
       <c r="L57" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M57" s="15"/>
+      <c r="M57" s="15" t="s">
+        <v>245</v>
+      </c>
       <c r="N57" s="11">
         <v>1</v>
       </c>
-      <c r="O57" s="11"/>
+      <c r="O57" s="11" t="s">
+        <v>201</v>
+      </c>
       <c r="P57" s="22" t="s">
         <v>163</v>
       </c>
@@ -4296,10 +4696,10 @@
       </c>
     </row>
     <row r="58" spans="2:18" s="27" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="47"/>
+      <c r="B58" s="33"/>
       <c r="C58" s="30"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="46"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="32"/>
     </row>
     <row r="59" spans="2:18" s="27" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="2:18" s="27" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>